<commit_message>
Updated df column names and references
</commit_message>
<xml_diff>
--- a/data/spreadsheets/live-targets.xlsx
+++ b/data/spreadsheets/live-targets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\web\svrel\finance-dashboard\data\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E070ED3F-2D42-409D-B726-D380B0E4FC5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B563042E-5910-4CCE-BEF7-75642D7C68D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="31920" xr2:uid="{F04729CC-D04B-42E0-942F-B943278F4BCC}"/>
+    <workbookView xWindow="1950" yWindow="1200" windowWidth="27855" windowHeight="31200" xr2:uid="{F04729CC-D04B-42E0-942F-B943278F4BCC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -421,7 +421,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,7 +539,7 @@
         <v>45292</v>
       </c>
       <c r="B14" s="1">
-        <v>1000000000</v>
+        <v>459193710.18150002</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -547,7 +547,7 @@
         <v>45323</v>
       </c>
       <c r="B15" s="1">
-        <v>1000000000</v>
+        <v>422540529.20887506</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -555,7 +555,7 @@
         <v>45352</v>
       </c>
       <c r="B16" s="1">
-        <v>1000000000</v>
+        <v>137691163.72475001</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -563,7 +563,7 @@
         <v>45383</v>
       </c>
       <c r="B17" s="1">
-        <v>1000000000</v>
+        <v>552065941.25979996</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -571,7 +571,7 @@
         <v>45413</v>
       </c>
       <c r="B18" s="1">
-        <v>1000000000</v>
+        <v>527964562.28925002</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -579,7 +579,7 @@
         <v>45444</v>
       </c>
       <c r="B19" s="1">
-        <v>1000000000</v>
+        <v>545770222.41162503</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -587,7 +587,7 @@
         <v>45474</v>
       </c>
       <c r="B20" s="1">
-        <v>1000000000</v>
+        <v>428309905.52437502</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -595,7 +595,7 @@
         <v>45505</v>
       </c>
       <c r="B21" s="1">
-        <v>1000000000</v>
+        <v>592410547.87699997</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -603,7 +603,7 @@
         <v>45536</v>
       </c>
       <c r="B22" s="1">
-        <v>1000000000</v>
+        <v>445800000</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -611,7 +611,7 @@
         <v>45566</v>
       </c>
       <c r="B23" s="1">
-        <v>1000000000</v>
+        <v>514956287.90000004</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -619,7 +619,7 @@
         <v>45597</v>
       </c>
       <c r="B24" s="1">
-        <v>1000000000</v>
+        <v>508654001.75</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -627,7 +627,7 @@
         <v>45627</v>
       </c>
       <c r="B25" s="1">
-        <v>1000000000</v>
+        <v>548376614.64999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>